<commit_message>
poprawka do ładowania rund
</commit_message>
<xml_diff>
--- a/testresources/matchRound.xlsx
+++ b/testresources/matchRound.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Typer\testresources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6C6D2B5-A1F8-4400-9B0A-1854BCC7C5F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC2FE49-ECD2-4C51-B7D1-24B8CD95BB9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="8726" xr2:uid="{EC39A77A-7552-4B38-829B-15AD33865FEF}"/>
   </bookViews>
@@ -35,10 +35,10 @@
     <t>name</t>
   </si>
   <si>
-    <t>roundId</t>
+    <t>runda1</t>
   </si>
   <si>
-    <t>runda1</t>
+    <t>leagueId</t>
   </si>
 </sst>
 </file>
@@ -406,7 +406,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -420,12 +420,12 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>2</v>

</xml_diff>